<commit_message>
Changing graph to average number of keypoints detected per image
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenpower/Development/GitHub Projects/SensorFusion-Projects/SensorFusionND-Camera-FeatureTracking/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FE2FCE-78D6-8A40-87D3-32984A1C2481}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6132B6E8-2367-4D49-AE1F-720B55C267AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="4820" windowWidth="37940" windowHeight="21280" xr2:uid="{5CF3A7BF-E245-9F47-8734-92F7C93A74E7}"/>
+    <workbookView xWindow="9620" yWindow="4820" windowWidth="37940" windowHeight="21280" activeTab="1" xr2:uid="{5CF3A7BF-E245-9F47-8734-92F7C93A74E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Per0image keypoints" sheetId="1" r:id="rId1"/>
@@ -20,140 +20,116 @@
     <sheet name="Perf Eval 3b" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Per0image keypoints'!$A$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Per0image keypoints'!$A$3</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Per0image keypoints'!$B$4:$L$4</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Per0image keypoints'!$B$5:$L$5</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Per0image keypoints'!$B$6:$L$6</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Per0image keypoints'!$B$7:$L$7</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Per0image keypoints'!$B$8:$L$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Per0image keypoints'!$A$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Per0image keypoints'!$A$5</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Per0image keypoints'!$A$6</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Per0image keypoints'!$A$7</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Per0image keypoints'!$A$8</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Per0image keypoints'!$B$1:$L$1</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Per0image keypoints'!$B$2:$L$2</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">'Perf Eval 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">'Perf Eval 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Per0image keypoints'!$B$3:$L$3</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">'Perf Eval 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">'Perf Eval 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">'Perf Eval 2'!$B$1</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">'Perf Eval 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">'Per0image keypoints'!$A$2</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">'Per0image keypoints'!$A$3</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">'Per0image keypoints'!$A$4</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">'Per0image keypoints'!$A$5</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">'Per0image keypoints'!$A$6</definedName>
-    <definedName name="_xlchart.v2.20" hidden="1">'Per0image keypoints'!$A$7</definedName>
-    <definedName name="_xlchart.v2.21" hidden="1">'Per0image keypoints'!$A$8</definedName>
-    <definedName name="_xlchart.v2.22" hidden="1">'Per0image keypoints'!$B$1:$L$1</definedName>
-    <definedName name="_xlchart.v2.23" hidden="1">'Per0image keypoints'!$B$2:$L$2</definedName>
-    <definedName name="_xlchart.v2.24" hidden="1">'Per0image keypoints'!$B$3:$L$3</definedName>
-    <definedName name="_xlchart.v2.25" hidden="1">'Per0image keypoints'!$B$4:$L$4</definedName>
-    <definedName name="_xlchart.v2.26" hidden="1">'Per0image keypoints'!$B$5:$L$5</definedName>
-    <definedName name="_xlchart.v2.27" hidden="1">'Per0image keypoints'!$B$6:$L$6</definedName>
-    <definedName name="_xlchart.v2.28" hidden="1">'Per0image keypoints'!$B$7:$L$7</definedName>
-    <definedName name="_xlchart.v2.29" hidden="1">'Per0image keypoints'!$B$8:$L$8</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.104" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.105" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.106" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.107" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.108" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.109" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Perf Eval 1'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Perf Eval 1'!$B$1</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Perf Eval 1'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">'Perf Eval 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Perf Eval 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">'Perf Eval 2'!$D$2:$D$8</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">'Perf Eval 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">'Perf Eval 2'!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">'Perf Eval 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">'Perf Eval 2'!$F$2:$F$8</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">'Perf Eval 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">'Perf Eval 2'!$G$2:$G$8</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">'Perf Eval 2'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">'Perf Eval 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">'Perf Eval 2'!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'Perf Eval 1'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Perf Eval 1'!$B$1</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Perf Eval 1'!$B$2:$B$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -245,7 +221,7 @@
     <t>Detector</t>
   </si>
   <si>
-    <t>Keypoints on Preceding Vehicle</t>
+    <t>Average number of keypoints detected per image</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1412,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Keypoints on Preceding Vehicle</c:v>
+                  <c:v>Average number of keypoints detected per image</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1484,35 +1460,35 @@
             <c:numRef>
               <c:f>'Perf Eval 1'!$B$2:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13423</c:v>
+                  <c:v>1342</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1737</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17874</c:v>
+                  <c:v>1787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27116</c:v>
+                  <c:v>2711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13430</c:v>
+                  <c:v>1343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13861</c:v>
+                  <c:v>1386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-394F-4C4A-9408-FA590766E841}"/>
+              <c16:uniqueId val="{00000000-517C-504B-8246-A0F4C3502B6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1526,11 +1502,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1487400303"/>
-        <c:axId val="1487573839"/>
+        <c:axId val="1490697615"/>
+        <c:axId val="1490656623"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1487400303"/>
+        <c:axId val="1490697615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1487573839"/>
+        <c:crossAx val="1490656623"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1581,7 +1557,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1487573839"/>
+        <c:axId val="1490656623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1577,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1632,7 +1608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1487400303"/>
+        <c:crossAx val="1490697615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7051,22 +7027,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>711200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2C4CC39-FDDB-BF49-8F3D-FEE351DB1B08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C722297C-28A6-4149-8A63-17F640390773}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7509,8 +7485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4B78F5-9055-5043-8F13-533D92D884FD}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7836,14 +7812,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195A1A87-6C31-D84E-BB59-6ACE872785DD}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -7858,56 +7833,56 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3">
-        <v>13423</v>
+      <c r="B2">
+        <v>1342</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
-        <v>1737</v>
+      <c r="B3">
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3">
-        <v>17874</v>
+      <c r="B4">
+        <v>1787</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
-        <v>27116</v>
+      <c r="B5">
+        <v>2711</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3">
-        <v>5000</v>
+      <c r="B6">
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3">
-        <v>13430</v>
+      <c r="B7">
+        <v>1343</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3">
-        <v>13861</v>
+      <c r="B8">
+        <v>1386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding recommendations, and additional notes
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenpower/Development/GitHub Projects/SensorFusion-Projects/SensorFusionND-Camera-FeatureTracking/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6132B6E8-2367-4D49-AE1F-720B55C267AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2921DD4D-BFFB-6247-A88C-5790D35B875B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="4820" windowWidth="37940" windowHeight="21280" activeTab="1" xr2:uid="{5CF3A7BF-E245-9F47-8734-92F7C93A74E7}"/>
+    <workbookView xWindow="56940" yWindow="4720" windowWidth="37940" windowHeight="21280" activeTab="5" xr2:uid="{5CF3A7BF-E245-9F47-8734-92F7C93A74E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Per0image keypoints" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Perf Eval 2" sheetId="3" r:id="rId3"/>
     <sheet name="Perf Eval 3a" sheetId="4" r:id="rId4"/>
     <sheet name="Perf Eval 3b" sheetId="6" r:id="rId5"/>
+    <sheet name="Perf Eval 3a+b" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.10" hidden="1">'Perf Eval 2'!$C$2:$C$8</definedName>
@@ -130,6 +131,7 @@
     <definedName name="_xlchart.v2.0" hidden="1">'Perf Eval 1'!$A$2:$A$8</definedName>
     <definedName name="_xlchart.v2.1" hidden="1">'Perf Eval 1'!$B$1</definedName>
     <definedName name="_xlchart.v2.2" hidden="1">'Perf Eval 1'!$B$2:$B$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Perf Eval 3a+b'!$A$1:$V$10</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -150,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
   <si>
     <t>Keypoint Detector</t>
   </si>
@@ -223,6 +225,18 @@
   <si>
     <t>Average number of keypoints detected per image</t>
   </si>
+  <si>
+    <t>Descriptor Extraction Times</t>
+  </si>
+  <si>
+    <t>Keypoint Detection Times</t>
+  </si>
+  <si>
+    <t>Total Time (Keypoint detection + Descriptor extraction)</t>
+  </si>
+  <si>
+    <t>Descriptor</t>
+  </si>
 </sst>
 </file>
 
@@ -248,15 +262,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -264,15 +302,109 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7804,6 +7936,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -7812,8 +7945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195A1A87-6C31-D84E-BB59-6ACE872785DD}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A1:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7887,6 +8020,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -7932,20 +8066,20 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>767</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>944</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>1814</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>766</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4">
         <v>926</v>
       </c>
     </row>
@@ -7953,20 +8087,20 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>142</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>173</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>320</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>146</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4">
         <v>163</v>
       </c>
     </row>
@@ -7974,20 +8108,20 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>899</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1099</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>2162</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>881</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4">
         <v>1048</v>
       </c>
     </row>
@@ -7995,20 +8129,20 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>1570</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>1704</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>3020</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>1526</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
         <v>1662</v>
       </c>
     </row>
@@ -8016,20 +8150,20 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>751</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>545</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>1522</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>421</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4">
         <v>765</v>
       </c>
     </row>
@@ -8037,22 +8171,22 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>1215</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>1266</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>2372</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>1188</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>2518</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
         <v>1273</v>
       </c>
     </row>
@@ -8060,23 +8194,24 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>304</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>338</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
         <v>274</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
         <v>801</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -8086,7 +8221,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G8" sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8121,20 +8256,20 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>113.961</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>103.28100000000001</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>182.74600000000001</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>88.676100000000005</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>88.658100000000005</v>
       </c>
     </row>
@@ -8142,20 +8277,20 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>117.739</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>115.977</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>224.02600000000001</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>114.51900000000001</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>120.658</v>
       </c>
     </row>
@@ -8163,20 +8298,20 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>2.75996</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>2.8483399999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>5.5042499999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>2.7440799999999999</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>2.7458100000000001</v>
       </c>
     </row>
@@ -8184,20 +8319,20 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>49.294899999999998</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>49.344900000000003</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>103.928</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>51.104100000000003</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>49.984699999999997</v>
       </c>
     </row>
@@ -8205,20 +8340,20 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>17.722000000000001</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>13.3629</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>20.6844</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>11.459099999999999</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
         <v>12.404400000000001</v>
       </c>
     </row>
@@ -8226,22 +8361,22 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>170.732</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>174.56200000000001</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>340.93900000000002</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>175.43799999999999</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>368.82499999999999</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>183.47</v>
       </c>
     </row>
@@ -8249,23 +8384,24 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>251.05099999999999</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>247.2</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
         <v>244.24700000000001</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
         <v>260.25900000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -8275,7 +8411,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G8" sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8310,20 +8446,20 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>16.044799999999999</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>8.9152500000000003</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>40.135100000000001</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>164.88300000000001</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>108.667</v>
       </c>
     </row>
@@ -8331,20 +8467,20 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>9.7620699999999996</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>5.4260299999999999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>41.2102</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>155.613</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>123.167</v>
       </c>
     </row>
@@ -8352,20 +8488,20 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>8.5435800000000004</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>3.6815500000000001</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>18.1524</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>80.790099999999995</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>57.061700000000002</v>
       </c>
     </row>
@@ -8373,20 +8509,20 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>4.3043899999999997</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>2.0322499999999999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>21.360199999999999</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>27.7593</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>31.648099999999999</v>
       </c>
     </row>
@@ -8394,20 +8530,20 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>3.0060099999999998</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>2.8468</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>25.0946</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>31.445399999999999</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
         <v>59.413699999999999</v>
       </c>
     </row>
@@ -8415,22 +8551,22 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>8.5550599999999992</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>4.4271599999999998</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>32.1053</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>43.9621</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>311.096</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>67.972999999999999</v>
       </c>
     </row>
@@ -8438,23 +8574,599 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>6.2278000000000002</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>5.2670399999999997</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
         <v>55.579599999999999</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
         <v>197.059</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0FADC3-5574-5C4F-971C-1A80C46413A2}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" customWidth="1"/>
+    <col min="16" max="16" width="2.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="Q1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+    </row>
+    <row r="2" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="16"/>
+    </row>
+    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="16"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18">
+        <v>113.961</v>
+      </c>
+      <c r="D4" s="2">
+        <v>103.28100000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>182.74600000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>88.676100000000005</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>88.658100000000005</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="2">
+        <v>16.044799999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>8.9152500000000003</v>
+      </c>
+      <c r="L4" s="2">
+        <v>40.135100000000001</v>
+      </c>
+      <c r="M4" s="2">
+        <v>164.88300000000001</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2">
+        <v>108.667</v>
+      </c>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="5">
+        <f>C4+J4</f>
+        <v>130.00579999999999</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:V4" si="0">D4+K4</f>
+        <v>112.19625000000001</v>
+      </c>
+      <c r="S4" s="5">
+        <f t="shared" si="0"/>
+        <v>222.8811</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" si="0"/>
+        <v>253.5591</v>
+      </c>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5">
+        <f t="shared" si="0"/>
+        <v>197.32510000000002</v>
+      </c>
+      <c r="W4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="18">
+        <v>117.739</v>
+      </c>
+      <c r="D5" s="2">
+        <v>115.977</v>
+      </c>
+      <c r="E5" s="2">
+        <v>224.02600000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>114.51900000000001</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>120.658</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" s="2">
+        <v>9.7620699999999996</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5.4260299999999999</v>
+      </c>
+      <c r="L5" s="2">
+        <v>41.2102</v>
+      </c>
+      <c r="M5" s="2">
+        <v>155.613</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
+        <v>123.167</v>
+      </c>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="5">
+        <f t="shared" ref="Q5:Q10" si="1">C5+J5</f>
+        <v>127.50107</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" ref="R5:R10" si="2">D5+K5</f>
+        <v>121.40303</v>
+      </c>
+      <c r="S5" s="5">
+        <f t="shared" ref="S5:S9" si="3">E5+L5</f>
+        <v>265.2362</v>
+      </c>
+      <c r="T5" s="5">
+        <f t="shared" ref="T5:T10" si="4">F5+M5</f>
+        <v>270.13200000000001</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
+        <f t="shared" ref="V5:V10" si="5">H5+O5</f>
+        <v>243.82499999999999</v>
+      </c>
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2.75996</v>
+      </c>
+      <c r="D6" s="24">
+        <v>2.8483399999999999</v>
+      </c>
+      <c r="E6" s="24">
+        <v>5.5042499999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.7440799999999999</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>2.7458100000000001</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="24">
+        <v>8.5435800000000004</v>
+      </c>
+      <c r="K6" s="24">
+        <v>3.6815500000000001</v>
+      </c>
+      <c r="L6" s="24">
+        <v>18.1524</v>
+      </c>
+      <c r="M6" s="2">
+        <v>80.790099999999995</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
+        <v>57.061700000000002</v>
+      </c>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="20">
+        <f t="shared" si="1"/>
+        <v>11.30354</v>
+      </c>
+      <c r="R6" s="20">
+        <f t="shared" si="2"/>
+        <v>6.52989</v>
+      </c>
+      <c r="S6" s="22">
+        <f t="shared" si="3"/>
+        <v>23.656649999999999</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" si="4"/>
+        <v>83.534179999999992</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5">
+        <f t="shared" si="5"/>
+        <v>59.807510000000001</v>
+      </c>
+      <c r="W6" s="11"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="18">
+        <v>49.294899999999998</v>
+      </c>
+      <c r="D7" s="2">
+        <v>49.344900000000003</v>
+      </c>
+      <c r="E7" s="2">
+        <v>103.928</v>
+      </c>
+      <c r="F7" s="2">
+        <v>51.104100000000003</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>49.984699999999997</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="2">
+        <v>4.3043899999999997</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.0322499999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>21.360199999999999</v>
+      </c>
+      <c r="M7" s="2">
+        <v>27.7593</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
+        <v>31.648099999999999</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="5">
+        <f t="shared" si="1"/>
+        <v>53.599289999999996</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="2"/>
+        <v>51.37715</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="3"/>
+        <v>125.28819999999999</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="4"/>
+        <v>78.863399999999999</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5">
+        <f t="shared" si="5"/>
+        <v>81.632800000000003</v>
+      </c>
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="23">
+        <v>17.722000000000001</v>
+      </c>
+      <c r="D8" s="24">
+        <v>13.3629</v>
+      </c>
+      <c r="E8" s="2">
+        <v>20.6844</v>
+      </c>
+      <c r="F8" s="2">
+        <v>11.459099999999999</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>12.404400000000001</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="24">
+        <v>3.0060099999999998</v>
+      </c>
+      <c r="K8" s="24">
+        <v>2.8468</v>
+      </c>
+      <c r="L8" s="2">
+        <v>25.0946</v>
+      </c>
+      <c r="M8" s="2">
+        <v>31.445399999999999</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
+        <v>59.413699999999999</v>
+      </c>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="22">
+        <f t="shared" si="1"/>
+        <v>20.728010000000001</v>
+      </c>
+      <c r="R8" s="20">
+        <f t="shared" si="2"/>
+        <v>16.209699999999998</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="3"/>
+        <v>45.778999999999996</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="4"/>
+        <v>42.904499999999999</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5">
+        <f t="shared" si="5"/>
+        <v>71.818100000000001</v>
+      </c>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="18">
+        <v>170.732</v>
+      </c>
+      <c r="D9" s="2">
+        <v>174.56200000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>340.93900000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>175.43799999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <v>368.82499999999999</v>
+      </c>
+      <c r="H9" s="2">
+        <v>183.47</v>
+      </c>
+      <c r="I9" s="19"/>
+      <c r="J9" s="2">
+        <v>8.5550599999999992</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4.4271599999999998</v>
+      </c>
+      <c r="L9" s="2">
+        <v>32.1053</v>
+      </c>
+      <c r="M9" s="2">
+        <v>43.9621</v>
+      </c>
+      <c r="N9" s="2">
+        <v>311.096</v>
+      </c>
+      <c r="O9" s="2">
+        <v>67.972999999999999</v>
+      </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="5">
+        <f t="shared" si="1"/>
+        <v>179.28706</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="2"/>
+        <v>178.98916</v>
+      </c>
+      <c r="S9" s="5">
+        <f t="shared" si="3"/>
+        <v>373.04430000000002</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="4"/>
+        <v>219.40009999999998</v>
+      </c>
+      <c r="U9" s="21">
+        <f t="shared" ref="U9" si="6">G9+N9</f>
+        <v>679.92100000000005</v>
+      </c>
+      <c r="V9" s="5">
+        <f t="shared" si="5"/>
+        <v>251.44299999999998</v>
+      </c>
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="18">
+        <v>251.05099999999999</v>
+      </c>
+      <c r="D10" s="2">
+        <v>247.2</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>244.24700000000001</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>260.25900000000001</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="2">
+        <v>6.2278000000000002</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5.2670399999999997</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2">
+        <v>55.579599999999999</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2">
+        <v>197.059</v>
+      </c>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="5">
+        <f t="shared" si="1"/>
+        <v>257.27879999999999</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="2"/>
+        <v>252.46704</v>
+      </c>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5">
+        <f t="shared" si="4"/>
+        <v>299.82659999999998</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5">
+        <f t="shared" si="5"/>
+        <v>457.31799999999998</v>
+      </c>
+      <c r="W10" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>